<commit_message>
Thu Mar 19 15:22:32 MDT 2015
</commit_message>
<xml_diff>
--- a/Results/Validating_Signatures/ERK/ERK_Validation_Data.xlsx
+++ b/Results/Validating_Signatures/ERK/ERK_Validation_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="20" windowWidth="23620" windowHeight="15040" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="1000" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2639" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="325">
   <si>
     <t>ERK25/adap_adap</t>
   </si>
@@ -988,13 +988,22 @@
   </si>
   <si>
     <t>With pair wise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adap_adap and adap </t>
+  </si>
+  <si>
+    <t>goes down with high number of genes</t>
+  </si>
+  <si>
+    <t>lower number of genes higher the prediction correlations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1052,8 +1061,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1082,6 +1099,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1174,14 +1197,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1223,12 +1278,46 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1575,10 +1664,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="11000" ySplit="1320"/>
+      <selection activeCell="C36" sqref="C36"/>
+      <selection pane="topRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1672,7 +1765,7 @@
       <c r="A3" t="s">
         <v>279</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="39">
         <v>0.80447330447330401</v>
       </c>
       <c r="C3">
@@ -1724,7 +1817,7 @@
       <c r="D6" s="1">
         <v>0.95187590187590199</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="40">
         <v>0.99992784992785</v>
       </c>
       <c r="F6" s="1">
@@ -1773,7 +1866,7 @@
       <c r="F8">
         <v>0.96096681096681102</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="39">
         <v>0.76305916305916299</v>
       </c>
       <c r="H8">
@@ -1799,7 +1892,7 @@
       <c r="F9">
         <v>0.96168831168831204</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="39">
         <v>0.76082251082251096</v>
       </c>
       <c r="H9">
@@ -1869,7 +1962,7 @@
       <c r="I11" s="1">
         <v>0.90735930735930703</v>
       </c>
-      <c r="J11" s="38">
+      <c r="J11" s="39">
         <v>0.83982683982684003</v>
       </c>
       <c r="K11" s="1">
@@ -1904,7 +1997,7 @@
       <c r="I12" s="1">
         <v>0.89076479076479098</v>
       </c>
-      <c r="J12" s="38">
+      <c r="J12" s="39">
         <v>0.83181818181818201</v>
       </c>
       <c r="K12" s="40">
@@ -2142,7 +2235,7 @@
       <c r="O17" s="1">
         <v>0.84834054834054795</v>
       </c>
-      <c r="P17" s="38">
+      <c r="P17" s="39">
         <v>0.88968253968253996</v>
       </c>
       <c r="Q17" s="1">
@@ -2195,7 +2288,7 @@
       <c r="O18" s="1">
         <v>0.83896103896103902</v>
       </c>
-      <c r="P18" s="38">
+      <c r="P18" s="39">
         <v>0.88816738816738805</v>
       </c>
       <c r="Q18" s="1">
@@ -2319,7 +2412,7 @@
       <c r="R20">
         <v>0.96976911976911995</v>
       </c>
-      <c r="S20" s="38">
+      <c r="S20" s="39">
         <v>0.804040404040404</v>
       </c>
       <c r="T20">
@@ -2381,11 +2474,19 @@
       <c r="R21">
         <v>0.96572871572871599</v>
       </c>
-      <c r="S21" s="38">
+      <c r="S21" s="39">
         <v>0.79913419913419903</v>
       </c>
       <c r="T21">
         <v>0.99891774891774898</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="B22" s="39">
+        <v>0.80447330447330401</v>
+      </c>
+      <c r="G22" s="39">
+        <v>0.76305916305916299</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="18">
@@ -2399,6 +2500,18 @@
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
       <c r="H23" s="27"/>
+      <c r="J23" s="39">
+        <v>0.83181818181818201</v>
+      </c>
+      <c r="M23" s="38">
+        <v>0.65259740259740295</v>
+      </c>
+      <c r="P23" s="39">
+        <v>0.88968253968253996</v>
+      </c>
+      <c r="S23" s="41">
+        <v>0.79913419900000005</v>
+      </c>
     </row>
     <row r="24" spans="1:20" ht="18">
       <c r="A24" s="36" t="s">
@@ -2473,6 +2586,70 @@
       <c r="F30" s="32"/>
       <c r="G30" s="32"/>
       <c r="H30" s="33"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="B32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33" s="39">
+        <v>0.83181818181818201</v>
+      </c>
+      <c r="C33" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>50</v>
+      </c>
+      <c r="B34" s="39">
+        <v>0.88968253968253996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>75</v>
+      </c>
+      <c r="B35" s="41">
+        <v>0.79913419900000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>100</v>
+      </c>
+      <c r="B36" s="39">
+        <v>0.80447330447330401</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>200</v>
+      </c>
+      <c r="B38" s="39">
+        <v>0.76305916305916299</v>
+      </c>
+      <c r="C38" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>250</v>
+      </c>
+      <c r="B39" s="42">
+        <v>0.65259740300000002</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -18473,7 +18650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>

</xml_diff>